<commit_message>
update personal doc listing
</commit_message>
<xml_diff>
--- a/docs/personal/docs.xlsx
+++ b/docs/personal/docs.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">cv</t>
   </si>
   <si>
-    <t xml:space="preserve">Curriculum vitae</t>
+    <t xml:space="preserve">Curriculum Vitae</t>
   </si>
   <si>
     <t xml:space="preserve">Professional Documents</t>
@@ -195,10 +195,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.66"/>

</xml_diff>